<commit_message>
added project management part to final report
</commit_message>
<xml_diff>
--- a/documents/project management/project_management.xlsx
+++ b/documents/project management/project_management.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -528,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +543,7 @@
     <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -577,7 +577,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1.2</v>
       </c>
@@ -594,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2.2999999999999998</v>
       </c>
@@ -611,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1.4</v>
       </c>
@@ -627,8 +627,16 @@
       <c r="E5" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f>SUM(D2:D5)</f>
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <f>SUM(E2:E5)</f>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2.1</v>
       </c>
@@ -645,7 +653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -662,7 +670,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2.2999999999999998</v>
       </c>
@@ -678,8 +686,16 @@
       <c r="E8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <f>SUM(D6:D8)</f>
+        <v>34</v>
+      </c>
+      <c r="H8">
+        <f>SUM(E6:E8)</f>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>3.1</v>
       </c>
@@ -696,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>3.2</v>
       </c>
@@ -713,7 +729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>3.3</v>
       </c>
@@ -730,7 +746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>3.4</v>
       </c>
@@ -747,7 +763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>3.5</v>
       </c>
@@ -764,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>3.6</v>
       </c>
@@ -780,8 +796,16 @@
       <c r="E14" s="3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <f>SUM(D9:D14)</f>
+        <v>34</v>
+      </c>
+      <c r="H14">
+        <f>SUM(E9:E14)</f>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4.0999999999999996</v>
       </c>
@@ -798,7 +822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4.2</v>
       </c>
@@ -815,7 +839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4.3</v>
       </c>
@@ -832,7 +856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4.4000000000000004</v>
       </c>
@@ -849,7 +873,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4.5</v>
       </c>
@@ -866,7 +890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4.5999999999999996</v>
       </c>
@@ -883,7 +907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4.7</v>
       </c>
@@ -899,8 +923,16 @@
       <c r="E21">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <f>SUM(D15:D21)</f>
+        <v>43</v>
+      </c>
+      <c r="H21">
+        <f>SUM(E15:E21)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>5.0999999999999996</v>
       </c>
@@ -917,7 +949,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>5.2</v>
       </c>
@@ -934,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>5.3</v>
       </c>
@@ -951,7 +983,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>5.4</v>
       </c>
@@ -968,7 +1000,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>5.5</v>
       </c>
@@ -985,7 +1017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>5.6</v>
       </c>
@@ -1002,7 +1034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>5.7</v>
       </c>
@@ -1019,7 +1051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>5.8</v>
       </c>
@@ -1036,7 +1068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>5.9</v>
       </c>
@@ -1052,8 +1084,16 @@
       <c r="E30" s="3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <f>SUM(D22:D30)</f>
+        <v>74</v>
+      </c>
+      <c r="H30">
+        <f>SUM(E22:E30)</f>
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>6.1</v>
       </c>
@@ -1070,7 +1110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>6.2</v>
       </c>
@@ -1087,7 +1127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6.3</v>
       </c>
@@ -1104,7 +1144,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>6.4</v>
       </c>
@@ -1121,7 +1161,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6.5</v>
       </c>
@@ -1138,7 +1178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6.6</v>
       </c>
@@ -1155,7 +1195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6.7</v>
       </c>
@@ -1172,7 +1212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>6.8</v>
       </c>
@@ -1188,8 +1228,16 @@
       <c r="E38">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <f>SUM(D31:D38)</f>
+        <v>98</v>
+      </c>
+      <c r="H38">
+        <f>SUM(E31:E38)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="D40" s="2">
         <f>SUM(Table1[Expected Time '[h']])</f>
         <v>309</v>

</xml_diff>